<commit_message>
major changes to entire Mesopolis framework
</commit_message>
<xml_diff>
--- a/Input Files/Mesopolis_pop_at_node_kind.xlsx
+++ b/Input Files/Mesopolis_pop_at_node_kind.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squar\Documents\hydraulic_ABM\Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vizan/Documents/hydraulic_ABM/Input Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70B9C0D-B147-485D-A552-0DFD39121689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254CD89B-E6FB-E240-9EC2-9832F835B3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2715" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>t</t>
   </si>
@@ -56,11 +56,20 @@
   <si>
     <t>navy</t>
   </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>Savannah/Hilton Head Passengers 2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,10 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,21 +385,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10" hidden="1" customWidth="1"/>
+    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +427,7 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -422,26 +438,29 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
-        <v>1</v>
+      <c r="M1" t="s">
+        <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
@@ -462,37 +481,53 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2">
-        <f>N2/S27</f>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I2" s="2">
-        <f>C2/F2</f>
-        <v>0</v>
+        <f>O2/T27</f>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <f>I34/T27</f>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J2" s="2">
         <f>D2/F2</f>
         <v>0</v>
       </c>
       <c r="K2" s="2">
-        <f>E2/F2</f>
-        <v>0.76291793313069911</v>
+        <f>1-(H2+I2+J2+L2)</f>
+        <v>0.45413277784770023</v>
       </c>
       <c r="L2" s="2">
-        <f>R2/S27</f>
-        <v>0.49556967201941166</v>
-      </c>
-      <c r="N2">
-        <v>7062</v>
+        <f>S2/T27</f>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M2" s="2">
+        <f>SUM(H2:L2)</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>7062</v>
+      </c>
+      <c r="P2" s="1">
+        <f>ROUND(I2*$T$27,0)</f>
+        <v>317</v>
+      </c>
+      <c r="Q2">
+        <f>ROUND(J2*$T$27,0)</f>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>72708</v>
+        <f>ROUND(K2*$T$27,0)</f>
+        <v>66629</v>
       </c>
       <c r="S2">
-        <f>SUM(N2:R2)</f>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T2">
+        <f>SUM(O2:S2)</f>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -516,31 +551,50 @@
         <f>H2</f>
         <v>4.8133809536792173E-2</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I25" si="0">C3/F3</f>
-        <v>0</v>
+      <c r="I3" s="4">
+        <f>I2</f>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J25" si="1">D3/F3</f>
+        <f t="shared" ref="J3:J25" si="0">D3/F3</f>
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K25" si="2">E3/F3</f>
-        <v>0.76291793313069911</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="N3">
-        <v>7062</v>
+        <f t="shared" ref="K3:K25" si="1">1-(H3+I3+J3+L3)</f>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L3" s="2">
+        <f>L2</f>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:M25" si="2">SUM(H3:L3)</f>
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>7062</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P25" si="3">ROUND(I3*$T$27,0)</f>
+        <v>317</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q25" si="4">ROUND(J3*$T$27,0)</f>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>72708</v>
+        <f t="shared" ref="R3:R25" si="5">ROUND(K3*$T$27,0)</f>
+        <v>66629</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S25" si="3">SUM(N3:R3)</f>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T25" si="6">SUM(O3:S3)</f>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -561,34 +615,53 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H25" si="4">H3</f>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="H4:I25" si="7">H3</f>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="2"/>
-        <v>0.76291793313069911</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="N4">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L25" si="8">L3</f>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>7062</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S4">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -609,34 +682,53 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="0"/>
-        <v>6.2961354754667827E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.7566217976552323</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="N5">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>7062</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S5">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -657,34 +749,53 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>8.4672166739036044E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="2"/>
-        <v>0.75445071645679551</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="N6">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>7062</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S6">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -705,34 +816,53 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>8.4690553745928338E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.7752442996742671E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="2"/>
-        <v>0.68686210640608036</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="N7">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.38638033485095757</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>7062</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="4"/>
+        <v>9940</v>
       </c>
       <c r="R7">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>56688</v>
       </c>
       <c r="S7">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -753,34 +883,53 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1723838471558836E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.12700825010855407</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="2"/>
-        <v>0.62418584455058623</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="N8">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.32712452773914624</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>7062</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="4"/>
+        <v>18634</v>
       </c>
       <c r="R8">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>47994</v>
       </c>
       <c r="S8">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -801,34 +950,53 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2809379070777248E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.22709509335649153</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="2"/>
-        <v>0.52301346070343036</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="N9">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.22703768449120876</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>7062</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>33318</v>
       </c>
       <c r="R9">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>33310</v>
       </c>
       <c r="S9">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -849,34 +1017,53 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1723838471558836E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.32262266608771167</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="2"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="N10">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.13151011175998861</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>7062</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="4"/>
+        <v>47334</v>
       </c>
       <c r="R10">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>19295</v>
       </c>
       <c r="S10">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -897,34 +1084,53 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0638297872340425E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.40382110290924883</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.34845853234910984</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="N11">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>5.0311674938451456E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>7062</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>59247</v>
       </c>
       <c r="R11">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>7382</v>
       </c>
       <c r="S11">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -945,34 +1151,53 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2809379070777248E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.41597915762049503</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="2"/>
-        <v>0.33412939643942685</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="N12">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>3.8153620227205254E-2</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>7062</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="4"/>
+        <v>61031</v>
       </c>
       <c r="R12">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>5598</v>
       </c>
       <c r="S12">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -993,34 +1218,53 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="0"/>
-        <v>2.3447676943117671E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.44572297003907946</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="2"/>
-        <v>0.29374728614850193</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="N13">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>8.4098078086207728E-3</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>7062</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>65395</v>
       </c>
       <c r="R13">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>1234</v>
       </c>
       <c r="S13">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1041,34 +1285,53 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2362136343899261E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.44659140251845419</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.29396439426834564</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="N14">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>7.5413753292461472E-3</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>7062</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="4"/>
+        <v>65522</v>
       </c>
       <c r="R14">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>1106</v>
       </c>
       <c r="S14">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1089,34 +1352,53 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="0"/>
-        <v>1.910551454624403E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.44897959183673469</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="2"/>
-        <v>0.29483282674772038</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="N15">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>5.1531860109655936E-3</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>7062</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
+        <v>65872</v>
       </c>
       <c r="R15">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>756</v>
       </c>
       <c r="S15">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1137,34 +1419,53 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="0"/>
-        <v>1.8019973947025619E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4394268345636127</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.30547112462006076</v>
-      </c>
-      <c r="L16" s="2"/>
-      <c r="N16">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>1.4705943284087586E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>7062</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>64471</v>
       </c>
       <c r="R16">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>2158</v>
       </c>
       <c r="S16">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1185,34 +1486,53 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="0"/>
-        <v>1.715154146765089E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.42162396873643077</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="2"/>
-        <v>0.32414242292661744</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="N17">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>3.2508809111269521E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>7062</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>61859</v>
       </c>
       <c r="R17">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>4770</v>
       </c>
       <c r="S17">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1233,34 +1553,53 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="0"/>
-        <v>1.8019973947025619E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.38797221016066002</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="2"/>
-        <v>0.35692574902301344</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="N18">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>6.6160567687040261E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>7062</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="4"/>
+        <v>56922</v>
       </c>
       <c r="R18">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>9707</v>
       </c>
       <c r="S18">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1281,34 +1620,53 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.910551454624403E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31697785497177594</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.42683456361267913</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="N19">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.13715492287592435</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>7062</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>46506</v>
       </c>
       <c r="R19">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>20123</v>
       </c>
       <c r="S19">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1329,34 +1687,53 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="0"/>
-        <v>2.3447676943117671E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.22101606600086843</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.51845419018671302</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="N20">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.2331167118468318</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>7062</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="4"/>
+        <v>32427</v>
       </c>
       <c r="R20">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>34202</v>
       </c>
       <c r="S20">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1377,34 +1754,53 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="0"/>
-        <v>2.3447676943117671E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1326530612244898</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.60681719496309161</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="N21">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.32147971662321051</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>7062</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="4"/>
+        <v>19462</v>
       </c>
       <c r="R21">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>47166</v>
       </c>
       <c r="S21">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1425,34 +1821,53 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="0"/>
-        <v>1.910551454624403E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.7737733391228835E-2</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="2"/>
-        <v>0.67607468519322622</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="N22">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.38639504445647144</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>7062</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="4"/>
+        <v>9938</v>
       </c>
       <c r="R22">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>56690</v>
       </c>
       <c r="S22">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="6"/>
+        <v>146715</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1473,34 +1888,53 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2809379070777248E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="2"/>
-        <v>0.75010855405992183</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="N23">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>7062</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R23">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S23">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1521,34 +1955,53 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="0"/>
-        <v>6.2961354754667827E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.7566217976552323</v>
-      </c>
-      <c r="L24" s="2"/>
-      <c r="N24">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>7062</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R24">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S24">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72708</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="6"/>
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>11</v>
       </c>
@@ -1569,36 +2022,69 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="2">
-        <f t="shared" si="4"/>
-        <v>4.8133809536792173E-2</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="0"/>
-        <v>2.1710811984368217E-3</v>
+        <f t="shared" si="7"/>
+        <v>4.8133809536792173E-2</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="7"/>
+        <v>2.1637405960958835E-3</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="2"/>
-        <v>0.76074685193226221</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="N25">
-        <v>7062</v>
+        <f t="shared" si="1"/>
+        <v>0.45413277784770023</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49556967201941166</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>7062</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" si="3"/>
+        <v>317</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>72708</v>
+        <f t="shared" si="5"/>
+        <v>66629</v>
       </c>
       <c r="S25">
-        <f t="shared" si="3"/>
-        <v>79770</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S27">
+        <v>72708</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="6"/>
         <v>146716</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="T27">
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="3">
+        <v>2780909</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <f>I32/365/24</f>
+        <v>317.45536529680368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes to spreadsheets
</commit_message>
<xml_diff>
--- a/Input Files/Mesopolis_pop_at_node_kind.xlsx
+++ b/Input Files/Mesopolis_pop_at_node_kind.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vizan/Documents/hydraulic_ABM/Input Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE75B0-F2CA-A14B-8D4A-8B7E7691E8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E00C6-9DC9-2D47-BA41-4CC4541DCC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,15 +399,15 @@
   <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="9" width="8.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="14" width="8.83203125" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" customWidth="1"/>
+    <col min="2" max="9" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10" hidden="1" customWidth="1"/>
+    <col min="11" max="14" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="8.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>